<commit_message>
chore: Transpose columns in excel file
</commit_message>
<xml_diff>
--- a/data/openorders.xlsx
+++ b/data/openorders.xlsx
@@ -14,15 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ItemNo</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>Item1</t>
   </si>
   <si>
+    <t>This is item 1</t>
+  </si>
+  <si>
     <t>Item2</t>
+  </si>
+  <si>
+    <t>This is item 2</t>
   </si>
 </sst>
 </file>
@@ -391,87 +400,97 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="4" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
         <v>45444</v>
       </c>
-      <c r="C1" s="2">
+      <c r="D1" s="2">
         <v>45474</v>
       </c>
-      <c r="D1" s="2">
+      <c r="E1" s="2">
         <v>45505</v>
       </c>
-      <c r="E1" s="2">
+      <c r="F1" s="2">
         <v>45536</v>
       </c>
-      <c r="F1" s="2">
+      <c r="G1" s="2">
         <v>45566</v>
       </c>
-      <c r="G1" s="2">
+      <c r="H1" s="2">
         <v>45597</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3">
         <v>2000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>5000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>2500</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>3000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>2250</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>5250</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
         <v>3000</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>500</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>3000</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>3100</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>2500</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>1750</v>
       </c>
     </row>

</xml_diff>